<commit_message>
img fix  & place add
</commit_message>
<xml_diff>
--- a/data/m3_list_akb.xlsx
+++ b/data/m3_list_akb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -272,57 +272,58 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>r3</t>
+  </si>
+  <si>
+    <t>r4</t>
+  </si>
+  <si>
+    <t>r5</t>
+  </si>
+  <si>
+    <t>r6</t>
+  </si>
+  <si>
+    <t>r7</t>
+  </si>
+  <si>
+    <t>r8</t>
+  </si>
+  <si>
+    <t>r9</t>
+  </si>
+  <si>
+    <t>r10</t>
+  </si>
+  <si>
+    <t>gs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0226-36-3315</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>","</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>["</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"],</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>b11</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>r1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>r2</t>
-  </si>
-  <si>
-    <t>r3</t>
-  </si>
-  <si>
-    <t>r4</t>
-  </si>
-  <si>
-    <t>r5</t>
-  </si>
-  <si>
-    <t>r6</t>
-  </si>
-  <si>
-    <t>r7</t>
-  </si>
-  <si>
-    <t>r8</t>
-  </si>
-  <si>
-    <t>r9</t>
-  </si>
-  <si>
-    <t>r10</t>
-  </si>
-  <si>
-    <t>r11</t>
-  </si>
-  <si>
-    <t>gs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0226-36-3315</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>","</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>["</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>"],</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -402,8 +403,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -508,7 +547,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="115">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -547,6 +586,25 @@
     <cellStyle name="ハイパーリンク" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -586,6 +644,25 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="114" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -916,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -933,13 +1010,13 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="H1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" t="s">
         <v>88</v>
-      </c>
-      <c r="J1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="31">
@@ -949,8 +1026,8 @@
       <c r="B2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>75</v>
+      <c r="C2" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="D2" s="1">
         <v>141.56147569999999</v>
@@ -959,14 +1036,14 @@
         <v>38.699205499999998</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>44</v>
       </c>
       <c r="H2" t="str">
         <f>CONCATENATE($H$1,B2,$I$1,C2,$I$1,D2,$I$1,E2,$I$1,F2,$J$1)</f>
-        <v>["ニュー泊崎荘","r1","141.5614757","38.6992055","0226-36-3315"],</v>
+        <v>["ニュー泊崎荘","b1","141.5614757","38.6992055","0226-36-3315"],</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="31">
@@ -976,8 +1053,8 @@
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>76</v>
+      <c r="C3" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="D3" s="1">
         <v>141.5590727</v>
@@ -993,7 +1070,7 @@
       </c>
       <c r="H3" t="str">
         <f t="shared" ref="H3:H24" si="0">CONCATENATE($H$1,B3,$I$1,C3,$I$1,D3,$I$1,E3,$I$1,F3,$J$1)</f>
-        <v>["民宿　清観荘","r2","141.5590727","38.7055659","0226-36-2414"],</v>
+        <v>["民宿　清観荘","b2","141.5590727","38.7055659","0226-36-2414"],</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="31">
@@ -1003,8 +1080,8 @@
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>77</v>
+      <c r="C4" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="D4" s="1">
         <v>141.52230499999999</v>
@@ -1020,7 +1097,7 @@
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
-        <v>["平成の森　宿泊施設","r3","141.522305","38.7169443","0226-36-3115"],</v>
+        <v>["平成の森　宿泊施設","b3","141.522305","38.7169443","0226-36-3115"],</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="31">
@@ -1030,8 +1107,8 @@
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>78</v>
+      <c r="C5" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="D5" s="1">
         <v>141.5227051</v>
@@ -1047,7 +1124,7 @@
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
-        <v>["農漁家民宿　やすらぎ","r4","141.5227051","38.7109226","0226-36-3670"],</v>
+        <v>["農漁家民宿　やすらぎ","b4","141.5227051","38.7109226","0226-36-3670"],</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="31">
@@ -1057,8 +1134,8 @@
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>79</v>
+      <c r="C6" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="D6" s="1">
         <v>141.42410949999999</v>
@@ -1074,7 +1151,7 @@
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
-        <v>["校舎の宿　さんさん館","r5","141.4241095","38.7184107","0226-46-5633"],</v>
+        <v>["校舎の宿　さんさん館","b5","141.4241095","38.7184107","0226-46-5633"],</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="31">
@@ -1084,8 +1161,8 @@
       <c r="B7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>80</v>
+      <c r="C7" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="D7" s="1">
         <v>141.40918400000001</v>
@@ -1101,7 +1178,7 @@
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
-        <v>["南三陸まなびの里　いりやど","r6","141.409184","38.7016757","0226-25-9501"],</v>
+        <v>["南三陸まなびの里　いりやど","b6","141.409184","38.7016757","0226-25-9501"],</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="31">
@@ -1111,8 +1188,8 @@
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>81</v>
+      <c r="C8" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="D8" s="1">
         <v>141.46763899999999</v>
@@ -1128,7 +1205,7 @@
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
-        <v>["民宿　下道荘","r7","141.467639","38.6766107","0226-46-6318"],</v>
+        <v>["民宿　下道荘","b7","141.467639","38.6766107","0226-46-6318"],</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="31">
@@ -1138,8 +1215,8 @@
       <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>82</v>
+      <c r="C9" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="D9" s="1">
         <v>141.4685862</v>
@@ -1155,7 +1232,7 @@
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
-        <v>["民宿　なか","r8","141.4685862","38.6763801","0226-46-6309"],</v>
+        <v>["民宿　なか","b8","141.4685862","38.6763801","0226-46-6309"],</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="31">
@@ -1165,8 +1242,8 @@
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>83</v>
+      <c r="C10" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="D10" s="1">
         <v>141.44757759999999</v>
@@ -1182,7 +1259,7 @@
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
-        <v>["南三陸ホテル観洋","r9","141.4475776","38.659651","0226-46-2442"],</v>
+        <v>["南三陸ホテル観洋","b9","141.4475776","38.659651","0226-46-2442"],</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="31">
@@ -1192,8 +1269,8 @@
       <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>84</v>
+      <c r="C11" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="D11" s="1">
         <v>141.4815562</v>
@@ -1209,7 +1286,7 @@
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
-        <v>["民宿　津の宮荘","r10","141.4815562","38.6424979","0226-46-9354"],</v>
+        <v>["民宿　津の宮荘","b10","141.4815562","38.6424979","0226-46-9354"],</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="31">
@@ -1220,7 +1297,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D12" s="1">
         <v>141.5089734</v>
@@ -1236,7 +1313,7 @@
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
-        <v>["民宿　ながしず荘","r11","141.5089734","38.6373437","0226-46-9248"],</v>
+        <v>["民宿　ながしず荘","b11","141.5089734","38.6373437","0226-46-9248"],</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1247,7 +1324,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D13" s="1">
         <v>141.5304988</v>
@@ -1263,7 +1340,7 @@
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
-        <v>["南三陸 竜巳や","b1","141.5304988","38.7190638","0226-25-9377"],</v>
+        <v>["南三陸 竜巳や","r1","141.5304988","38.7190638","0226-25-9377"],</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1274,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D14" s="1">
         <v>141.46389149999999</v>
@@ -1290,7 +1367,7 @@
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
-        <v>["山内鮮魚店　静江館","b2","141.4638915","38.6853097","0226-46-2159"],</v>
+        <v>["山内鮮魚店　静江館","r2","141.4638915","38.6853097","0226-46-2159"],</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1301,13 +1378,13 @@
         <v>24</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D15" s="1">
-        <v>141.437473297119</v>
+        <v>141.43781661987299</v>
       </c>
       <c r="E15" s="1">
-        <v>38.686581727166697</v>
+        <v>38.686313736883598</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>25</v>
@@ -1317,7 +1394,7 @@
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
-        <v>["創菜旬魚　はしもと","b3","141.437473297119","38.6865817271667","0226-29-6343"],</v>
+        <v>["創菜旬魚　はしもと","r3","141.437816619873","38.6863137368836","0226-29-6343"],</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1328,13 +1405,13 @@
         <v>26</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D16" s="1">
-        <v>141.437473297119</v>
+        <v>141.43927574157701</v>
       </c>
       <c r="E16" s="1">
-        <v>38.686581727166697</v>
+        <v>38.686313736883598</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>27</v>
@@ -1344,7 +1421,7 @@
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
-        <v>["松原食堂","b4","141.437473297119","38.6865817271667","0226-46-2433"],</v>
+        <v>["松原食堂","r4","141.439275741577","38.6863137368836","0226-46-2433"],</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1355,13 +1432,13 @@
         <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D17" s="1">
-        <v>141.437473297119</v>
+        <v>141.43601417541501</v>
       </c>
       <c r="E17" s="1">
-        <v>38.686581727166697</v>
+        <v>38.687184701633697</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>29</v>
@@ -1371,7 +1448,7 @@
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
-        <v>["季節料理　志のや","b5","141.437473297119","38.6865817271667","0226-47-1688"],</v>
+        <v>["季節料理　志のや","r5","141.436014175415","38.6871847016337","0226-47-1688"],</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1382,13 +1459,13 @@
         <v>30</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D18" s="1">
-        <v>141.437473297119</v>
+        <v>141.43464088439899</v>
       </c>
       <c r="E18" s="1">
-        <v>38.686581727166697</v>
+        <v>38.686715721931797</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>31</v>
@@ -1398,7 +1475,7 @@
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
-        <v>["豊楽食堂","b6","141.437473297119","38.6865817271667","0226-46-3512"],</v>
+        <v>["豊楽食堂","r6","141.434640884399","38.6867157219318","0226-46-3512"],</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1409,13 +1486,13 @@
         <v>32</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D19" s="1">
-        <v>141.437473297119</v>
+        <v>141.43549919128401</v>
       </c>
       <c r="E19" s="1">
-        <v>38.686581727166697</v>
+        <v>38.685509760012003</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>33</v>
@@ -1425,7 +1502,7 @@
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
-        <v>["弁慶鮨","b7","141.437473297119","38.6865817271667","0226-46-5141"],</v>
+        <v>["弁慶鮨","r7","141.435499191284","38.685509760012","0226-46-5141"],</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1436,13 +1513,13 @@
         <v>34</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D20" s="1">
-        <v>141.437473297119</v>
+        <v>141.440391540527</v>
       </c>
       <c r="E20" s="1">
-        <v>38.686581727166697</v>
+        <v>38.686313736883598</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>35</v>
@@ -1452,7 +1529,7 @@
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
-        <v>["三陸味処　田中前","b8","141.437473297119","38.6865817271667","0226-25-9937"],</v>
+        <v>["三陸味処　田中前","r8","141.440391540527","38.6863137368836","0226-25-9937"],</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1463,7 +1540,7 @@
         <v>36</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D21" s="1">
         <v>141.44757759999999</v>
@@ -1479,7 +1556,7 @@
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
-        <v>["南三陸観洋　レストランシーサイド","b9","141.4475776","38.659651","0226-46-2442"],</v>
+        <v>["南三陸観洋　レストランシーサイド","r9","141.4475776","38.659651","0226-46-2442"],</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1490,7 +1567,7 @@
         <v>37</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D22" s="1">
         <v>141.47686210000001</v>
@@ -1506,7 +1583,7 @@
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
-        <v>["オーイング菓子工房　Ryo","b10","141.4768621","38.6447586","090-9743-1333"],</v>
+        <v>["オーイング菓子工房　Ryo","r10","141.4768621","38.6447586","090-9743-1333"],</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1517,7 +1594,7 @@
         <v>56</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D23" s="1">
         <v>141.5164388</v>
@@ -1544,7 +1621,7 @@
         <v>59</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D24" s="1">
         <v>141.55558379999999</v>
@@ -1571,7 +1648,7 @@
         <v>62</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" s="1">
         <v>141.55665859999999</v>

</xml_diff>